<commit_message>
Angular new courses with all databinding and encapsulation
</commit_message>
<xml_diff>
--- a/Angular/ang_zaw.xlsx
+++ b/Angular/ang_zaw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repozytoria\Studies\Angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346CABEF-B310-4365-A6FD-8AB180A2E41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1152273B-9025-4FBF-A108-404B7C1BAA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2424" yWindow="1404" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="2565" windowWidth="11130" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>dependencies</t>
   </si>
@@ -108,7 +108,31 @@
     <t>oprócz</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>middleware</t>
+  </si>
+  <si>
+    <t>opogramowanie pośredniczące</t>
+  </si>
+  <si>
+    <t>populate</t>
+  </si>
+  <si>
+    <t>zaludniać/zasiedlać</t>
+  </si>
+  <si>
+    <t>colon</t>
+  </si>
+  <si>
+    <t>dwukropek</t>
+  </si>
+  <si>
+    <t>be aware of</t>
+  </si>
+  <si>
+    <t>crucial</t>
+  </si>
+  <si>
+    <t>kluczowy</t>
   </si>
 </sst>
 </file>
@@ -441,20 +465,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
-    <col min="2" max="2" width="80.77734375" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="80.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -482,7 +506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -496,7 +520,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -510,7 +534,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -524,7 +548,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -538,7 +562,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -552,9 +576,40 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
       <c r="D9" s="3" t="s">
-        <v>27</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ng-content - directive to display data in other components
</commit_message>
<xml_diff>
--- a/Angular/ang_zaw.xlsx
+++ b/Angular/ang_zaw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repozytoria\Studies\Angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1152273B-9025-4FBF-A108-404B7C1BAA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D729405-A4C9-4AB0-B445-673ED08F9771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="2565" windowWidth="11130" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1248" yWindow="1488" windowWidth="18120" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>dependencies</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>kluczowy</t>
+  </si>
+  <si>
+    <t>efficient</t>
+  </si>
+  <si>
+    <t>wydajny</t>
+  </si>
+  <si>
+    <t>get dumped</t>
+  </si>
+  <si>
+    <t>zostać porzuconym</t>
   </si>
 </sst>
 </file>
@@ -465,20 +477,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="80.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
+    <col min="2" max="2" width="80.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -506,7 +518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -520,7 +532,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -534,7 +546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -548,7 +560,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -562,7 +574,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -576,7 +588,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -590,7 +602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -604,12 +616,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>